<commit_message>
Gear connected and tested
</commit_message>
<xml_diff>
--- a/wiring 747-400.xlsx
+++ b/wiring 747-400.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="13395" windowHeight="5190" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="13395" windowHeight="5190" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Buttons" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="149">
   <si>
     <t>64BTN</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Qh164</t>
   </si>
   <si>
-    <t>0a</t>
-  </si>
-  <si>
     <t>Qh162</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
     <t>Qh407</t>
   </si>
   <si>
-    <t>0b</t>
-  </si>
-  <si>
     <t>RTPCenter</t>
   </si>
   <si>
@@ -211,12 +205,6 @@
     <t>Qh408</t>
   </si>
   <si>
-    <t>0c</t>
-  </si>
-  <si>
-    <t>0d</t>
-  </si>
-  <si>
     <t>M0/R3/b1</t>
   </si>
   <si>
@@ -284,6 +272,198 @@
   </si>
   <si>
     <t>DisplayRightOff</t>
+  </si>
+  <si>
+    <t>GPWS</t>
+  </si>
+  <si>
+    <t>GS</t>
+  </si>
+  <si>
+    <t>Flap</t>
+  </si>
+  <si>
+    <t>EHRFMC</t>
+  </si>
+  <si>
+    <t>EventRCD</t>
+  </si>
+  <si>
+    <t>EIUSelL</t>
+  </si>
+  <si>
+    <t>EIUSelAuto</t>
+  </si>
+  <si>
+    <t>EIUSelC</t>
+  </si>
+  <si>
+    <t>EIUSelR</t>
+  </si>
+  <si>
+    <t>HdgTrue</t>
+  </si>
+  <si>
+    <t>FMCL</t>
+  </si>
+  <si>
+    <t>FMCR</t>
+  </si>
+  <si>
+    <t>0x0011</t>
+  </si>
+  <si>
+    <t>0x0004</t>
+  </si>
+  <si>
+    <t>0x0005</t>
+  </si>
+  <si>
+    <t>0x000a</t>
+  </si>
+  <si>
+    <t>0x0006</t>
+  </si>
+  <si>
+    <t>0x0007</t>
+  </si>
+  <si>
+    <t>0x0008</t>
+  </si>
+  <si>
+    <t>0x0009</t>
+  </si>
+  <si>
+    <t>0x000b</t>
+  </si>
+  <si>
+    <t>0x000c</t>
+  </si>
+  <si>
+    <t>0x000d</t>
+  </si>
+  <si>
+    <t>0x0012</t>
+  </si>
+  <si>
+    <t>0x0013</t>
+  </si>
+  <si>
+    <t>0x0016</t>
+  </si>
+  <si>
+    <t>0x0014</t>
+  </si>
+  <si>
+    <t>0x0017</t>
+  </si>
+  <si>
+    <t>0x0015</t>
+  </si>
+  <si>
+    <t>Qh131</t>
+  </si>
+  <si>
+    <t>Qh132</t>
+  </si>
+  <si>
+    <t>Qh142</t>
+  </si>
+  <si>
+    <t>Qh143</t>
+  </si>
+  <si>
+    <t>0x0000</t>
+  </si>
+  <si>
+    <t>Qh165</t>
+  </si>
+  <si>
+    <t>Qh166</t>
+  </si>
+  <si>
+    <t>Qh167</t>
+  </si>
+  <si>
+    <t>PH7</t>
+  </si>
+  <si>
+    <t>PH8</t>
+  </si>
+  <si>
+    <t>PH9</t>
+  </si>
+  <si>
+    <t>32-Output</t>
+  </si>
+  <si>
+    <t>led_ARM</t>
+  </si>
+  <si>
+    <t>led_NOSE</t>
+  </si>
+  <si>
+    <t>led_WING</t>
+  </si>
+  <si>
+    <t>n.y.d.</t>
+  </si>
+  <si>
+    <t>led_GS</t>
+  </si>
+  <si>
+    <t>led_FLAP</t>
+  </si>
+  <si>
+    <t>led_GEAR</t>
+  </si>
+  <si>
+    <t>BrtUpr</t>
+  </si>
+  <si>
+    <t>BrtLwr</t>
+  </si>
+  <si>
+    <t>0x0018</t>
+  </si>
+  <si>
+    <t>Qh139</t>
+  </si>
+  <si>
+    <t>Qh141</t>
+  </si>
+  <si>
+    <t>0x0019</t>
+  </si>
+  <si>
+    <t>Rotary Device</t>
+  </si>
+  <si>
+    <t>M0/R1/b2</t>
+  </si>
+  <si>
+    <t>M0/R1/b1</t>
+  </si>
+  <si>
+    <t>M0/R1/b3</t>
+  </si>
+  <si>
+    <t>M0/R1/b4</t>
+  </si>
+  <si>
+    <t>M0/R1/b5</t>
+  </si>
+  <si>
+    <t>M0/R1/b7</t>
+  </si>
+  <si>
+    <t>M0/R1/b6</t>
+  </si>
+  <si>
+    <t>M0/R2/b1</t>
+  </si>
+  <si>
+    <t>M0/R2/b0</t>
   </si>
 </sst>
 </file>
@@ -656,10 +836,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +847,7 @@
     <col min="1" max="1" width="17.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="6.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
     <col min="6" max="6" width="11.140625" customWidth="1"/>
     <col min="7" max="7" width="11.7109375" customWidth="1"/>
@@ -687,7 +867,7 @@
         <v>12</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -700,8 +880,8 @@
       <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="D2">
-        <v>0</v>
+      <c r="D2" t="s">
+        <v>118</v>
       </c>
       <c r="E2" t="s">
         <v>14</v>
@@ -715,8 +895,8 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3">
-        <v>0</v>
+      <c r="D3" t="s">
+        <v>118</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -730,8 +910,8 @@
       <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="D4">
-        <v>0</v>
+      <c r="D4" t="s">
+        <v>118</v>
       </c>
       <c r="E4" t="s">
         <v>16</v>
@@ -745,8 +925,8 @@
       <c r="C5" t="s">
         <v>3</v>
       </c>
-      <c r="D5">
-        <v>0</v>
+      <c r="D5" t="s">
+        <v>118</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
@@ -760,8 +940,8 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6">
-        <v>0</v>
+      <c r="D6" t="s">
+        <v>118</v>
       </c>
       <c r="E6" t="s">
         <v>18</v>
@@ -775,8 +955,8 @@
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7">
-        <v>0</v>
+      <c r="D7" t="s">
+        <v>118</v>
       </c>
       <c r="E7" t="s">
         <v>19</v>
@@ -790,8 +970,8 @@
       <c r="C8" t="s">
         <v>3</v>
       </c>
-      <c r="D8">
-        <v>0</v>
+      <c r="D8" t="s">
+        <v>118</v>
       </c>
       <c r="E8" t="s">
         <v>20</v>
@@ -805,8 +985,8 @@
       <c r="C9" t="s">
         <v>3</v>
       </c>
-      <c r="D9">
-        <v>0</v>
+      <c r="D9" t="s">
+        <v>118</v>
       </c>
       <c r="E9" t="s">
         <v>21</v>
@@ -823,8 +1003,8 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D10">
-        <v>4</v>
+      <c r="D10" t="s">
+        <v>98</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
@@ -841,10 +1021,13 @@
       <c r="C11" t="s">
         <v>27</v>
       </c>
-      <c r="D11">
-        <v>5</v>
-      </c>
-      <c r="F11" s="3"/>
+      <c r="D11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" t="s">
+        <v>142</v>
+      </c>
+      <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -853,10 +1036,13 @@
       <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="F12" s="3"/>
+      <c r="D12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" t="s">
+        <v>143</v>
+      </c>
+      <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -865,24 +1051,30 @@
       <c r="C13" t="s">
         <v>27</v>
       </c>
-      <c r="D13">
-        <v>5</v>
-      </c>
-      <c r="F13" s="3"/>
+      <c r="D13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" t="s">
+        <v>144</v>
+      </c>
+      <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>100</v>
+      </c>
+      <c r="E14" t="s">
+        <v>145</v>
+      </c>
+      <c r="F14" s="1"/>
       <c r="G14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -892,10 +1084,13 @@
       <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="F15" s="3"/>
+      <c r="D15" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" t="s">
+        <v>140</v>
+      </c>
+      <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -910,10 +1105,13 @@
       <c r="C17" t="s">
         <v>35</v>
       </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
-      <c r="F17" s="3"/>
+      <c r="D17" t="s">
+        <v>101</v>
+      </c>
+      <c r="E17" t="s">
+        <v>141</v>
+      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
@@ -922,10 +1120,13 @@
       <c r="C18" t="s">
         <v>37</v>
       </c>
-      <c r="D18">
-        <v>7</v>
-      </c>
-      <c r="F18" s="3"/>
+      <c r="D18" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" t="s">
+        <v>148</v>
+      </c>
+      <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
@@ -934,12 +1135,15 @@
       <c r="C19" t="s">
         <v>40</v>
       </c>
-      <c r="D19">
-        <v>8</v>
-      </c>
-      <c r="F19" s="3"/>
+      <c r="D19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E19" t="s">
+        <v>146</v>
+      </c>
+      <c r="F19" s="1"/>
       <c r="G19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -949,363 +1153,507 @@
       <c r="C20" t="s">
         <v>41</v>
       </c>
-      <c r="D20">
-        <v>9</v>
-      </c>
-      <c r="F20" s="3"/>
+      <c r="D20" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" t="s">
+        <v>147</v>
+      </c>
+      <c r="F20" s="1"/>
       <c r="G20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" t="s">
         <v>48</v>
       </c>
-      <c r="B21" t="s">
-        <v>49</v>
-      </c>
       <c r="E21" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E23" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F23" s="1"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E24" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F27" s="1"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F28" s="1"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" t="s">
         <v>57</v>
       </c>
-      <c r="C29" t="s">
-        <v>58</v>
-      </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>105</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F29" s="1"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D31" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D33" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C34" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C36" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D37" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C38" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="F38" s="3"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F39" s="5"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D40" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F40" s="3"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D41" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F41" s="3"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F43" s="3"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C44" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F44" s="3"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C45" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D46" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F46" s="3"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C47" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
-        <v>65</v>
+        <v>107</v>
       </c>
       <c r="F47" s="3"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F48" s="5"/>
     </row>
-    <row r="49" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F49" s="5"/>
-    </row>
-    <row r="50" spans="6:6" x14ac:dyDescent="0.25">
-      <c r="F50" s="5"/>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B49" t="s">
+        <v>86</v>
+      </c>
+      <c r="C49" t="s">
+        <v>119</v>
+      </c>
+      <c r="D49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>87</v>
+      </c>
+      <c r="C50" t="s">
+        <v>120</v>
+      </c>
+      <c r="D50" t="s">
+        <v>108</v>
+      </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51" t="s">
+        <v>121</v>
+      </c>
+      <c r="D51" t="s">
+        <v>109</v>
+      </c>
+      <c r="F51" s="3"/>
+      <c r="G51" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" t="s">
+        <v>110</v>
+      </c>
+      <c r="F53" s="3"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>90</v>
+      </c>
+      <c r="C54" t="s">
+        <v>114</v>
+      </c>
+      <c r="D54" t="s">
+        <v>111</v>
+      </c>
+      <c r="F54" s="3"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>91</v>
+      </c>
+      <c r="C55" t="s">
+        <v>114</v>
+      </c>
+      <c r="D55" t="s">
+        <v>111</v>
+      </c>
+      <c r="F55" s="3"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>92</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" t="s">
+        <v>111</v>
+      </c>
+      <c r="F56" s="3"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C57" t="s">
+        <v>114</v>
+      </c>
+      <c r="D57" t="s">
+        <v>111</v>
+      </c>
+      <c r="F57" s="3"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" t="s">
+        <v>112</v>
+      </c>
+      <c r="F58" s="3"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>95</v>
+      </c>
+      <c r="C59" t="s">
+        <v>115</v>
+      </c>
+      <c r="D59" t="s">
+        <v>113</v>
+      </c>
+      <c r="F59" s="3"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" t="s">
+        <v>115</v>
+      </c>
+      <c r="D60" t="s">
+        <v>113</v>
+      </c>
+      <c r="F60" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1315,51 +1663,135 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="5" width="14.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
-        <v>4</v>
+        <v>125</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>60</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>130</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>8</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C14">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+      <c r="E14" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1368,10 +1800,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,6 +1811,7 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="13" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1390,32 +1823,110 @@
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>0</v>
+        <v>139</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
-        <v>49</v>
-      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>75</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" t="s">
+        <v>135</v>
+      </c>
+      <c r="E11">
+        <v>7</v>
+      </c>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D12" t="s">
+        <v>138</v>
+      </c>
+      <c r="E12">
+        <v>8</v>
+      </c>
+      <c r="F12" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1424,104 +1935,103 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12:D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B12" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>84</v>
       </c>
-      <c r="B12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>88</v>
-      </c>
+      <c r="D15" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>